<commit_message>
add FP and search_time
</commit_message>
<xml_diff>
--- a/docs/paper_experiment/FP/edit/edit_dist_time.xlsx
+++ b/docs/paper_experiment/FP/edit/edit_dist_time.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamadalab/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamadalab/.ghq/src/github.com/mitubaEX/research/docs/paper_experiment/FP/edit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C106336-9873-634D-8E90-2D318C8B9988}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9477AB46-3B91-F94B-A9F0-CC69C68B3920}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47520" yWindow="-8200" windowWidth="27900" windowHeight="16500" xr2:uid="{FD257585-9F5D-9545-ABF2-D9C714A598E5}"/>
+    <workbookView xWindow="31960" yWindow="-3600" windowWidth="27900" windowHeight="12760" activeTab="1" xr2:uid="{FD257585-9F5D-9545-ABF2-D9C714A598E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="比較" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>2gram</t>
     <phoneticPr fontId="2"/>
@@ -36,6 +37,14 @@
   </si>
   <si>
     <t>search_time</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>edit</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>BM25</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -93,11 +102,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -116,6 +131,1102 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>速度比</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>比較!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BM25</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>比較!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>比較!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.16494824381706938</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.13761175401229125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.14263135759927281</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13503411973789528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13781525145500673</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14595514916362551</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15925031542103618</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22009605079296171</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.44604604468803838</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.93671229531548894</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-86AF-424E-BC1B-4D9B9E3EB051}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>比較!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>edit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>比較!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>比較!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.8937300310500875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8940488437103413</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8951002471643719</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8978474626410309</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9200693833855595</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1081213701989254</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2067565806831135</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.2816029401138636</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3242085213703918</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.3002229561223286</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-86AF-424E-BC1B-4D9B9E3EB051}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1208730704"/>
+        <c:axId val="1208732400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1208730704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1208732400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1208732400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1208730704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>654050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="グラフ 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8745E41C-36A5-F04F-987A-7C410B06E74D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF6E024-7AB5-444F-BBCE-B3F5E20BFF98}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -647,4 +1758,139 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD8B884-6095-5D45-B45E-7CD90F6C185E}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0.9</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.16494824381706938</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4.8937300310500875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.13761175401229125</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.8940488437103413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.14263135759927281</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4.8951002471643719</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.13503411973789528</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.8978474626410309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.13781525145500673</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.9200693833855595</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.14595514916362551</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5.1081213701989254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.3</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.15925031542103618</v>
+      </c>
+      <c r="C8" s="2">
+        <v>5.2067565806831135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.22009605079296171</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5.2816029401138636</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.1</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.44604604468803838</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5.3242085213703918</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.93671229531548894</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5.3002229561223286</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>